<commit_message>
fix: bm25fr bugs & granularity merge merge ge in idx & report
</commit_message>
<xml_diff>
--- a/docs/exercise_03/Exercises_03_IR_indexing_weighting.xlsx
+++ b/docs/exercise_03/Exercises_03_IR_indexing_weighting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Documents\GitHub\zestones\information-retrieval\docs\exercise_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D9B107-AC1C-4EA3-82B3-000739F9D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A5BF5D-015C-40B2-8E06-679C01C67158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
     <definedName name="w_avdl_element">Feuil1!#REF!</definedName>
     <definedName name="w_avdl_title">Feuil1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1085,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -2958,6 +2958,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="K18:O18"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C8:G8"/>
@@ -2965,9 +2968,6 @@
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="C16:G16"/>
-    <mergeCell ref="K16:O16"/>
-    <mergeCell ref="K17:O17"/>
-    <mergeCell ref="K18:O18"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.15748031496062992" bottom="0.15748031496062992" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>